<commit_message>
Add data and updating util
</commit_message>
<xml_diff>
--- a/spreadsheets/segments.xlsx
+++ b/spreadsheets/segments.xlsx
@@ -33,7 +33,7 @@
     <t>00-00-00_00-15-00.mov</t>
   </si>
   <si>
-    <t>00-15-00_00-15-00.mov</t>
+    <t>00-15-00_00-30-00.mov</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Working on VideoConcatoner class
</commit_message>
<xml_diff>
--- a/spreadsheets/segments.xlsx
+++ b/spreadsheets/segments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>id</t>
   </si>
@@ -40,10 +40,28 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
@@ -67,13 +85,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -448,8 +470,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Working on front end
</commit_message>
<xml_diff>
--- a/spreadsheets/segments.xlsx
+++ b/spreadsheets/segments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="2620" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>00-15-00_00-30-00.mov</t>
+  </si>
+  <si>
+    <t>00-07-00_00-15-00.mov</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -475,10 +478,21 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin testing webcam server/client
</commit_message>
<xml_diff>
--- a/spreadsheets/segments.xlsx
+++ b/spreadsheets/segments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2620" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>id</t>
   </si>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -495,6 +495,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Temporarily using word_clips_h264 and -c:v copy to concatonate videos. Gives huge speed boost with a bit of a drop in quality.
</commit_message>
<xml_diff>
--- a/spreadsheets/segments.xlsx
+++ b/spreadsheets/segments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>00-45-00_00-58-00.mov</t>
+  </si>
+  <si>
+    <t>00-15-00_00-21-41.mov</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -546,6 +549,17 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>